<commit_message>
updated course programming raw data
</commit_message>
<xml_diff>
--- a/data/sum/asignaturas programadas xlsx/criminalistica.xlsx
+++ b/data/sum/asignaturas programadas xlsx/criminalistica.xlsx
@@ -1,34 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dev\Documents\data del sum\asignaturas programadas xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC MATRICULA\Desktop\data del sum\xlsx\asignaturas programadas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8B5FE4-7011-4705-887B-F02C02B0ADDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="105" windowWidth="13215" windowHeight="7005"/>
   </bookViews>
   <sheets>
     <sheet name="criminalistica" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -302,7 +288,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -416,53 +402,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F3F95F41-F5EA-40A8-A87E-F764A409A367}" name="Table1" displayName="Table1" ref="A1:AB15" totalsRowShown="0">
-  <autoFilter ref="A1:AB15" xr:uid="{F3F95F41-F5EA-40A8-A87E-F764A409A367}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AB15">
-    <sortCondition ref="N2:N15"/>
-    <sortCondition ref="C2:C15"/>
-    <sortCondition ref="A2:A15"/>
-    <sortCondition ref="L2:L15"/>
-  </sortState>
-  <tableColumns count="28">
-    <tableColumn id="1" xr3:uid="{AE6C6439-56C5-4326-B97F-3DEFC8A2F2C5}" name="cod_asignatura"/>
-    <tableColumn id="2" xr3:uid="{F9F7B01C-31A3-460C-90B8-5EDD15F2F07E}" name="cod_tipo_acta"/>
-    <tableColumn id="3" xr3:uid="{1D01ED24-BD2B-4287-A117-256929710B73}" name="cod_seccion"/>
-    <tableColumn id="4" xr3:uid="{5BD464BB-0699-4CF0-B0D6-C7A8FDE30BC9}" name="cod_turno"/>
-    <tableColumn id="5" xr3:uid="{1B44619F-29DA-4D27-A05E-66CDC07DCFD0}" name="can_tope_alumnos"/>
-    <tableColumn id="6" xr3:uid="{E304488C-7BD6-4F4E-A443-559E984733A3}" name="cod_facultad"/>
-    <tableColumn id="7" xr3:uid="{D629FA5B-6DCD-4D49-9667-2B6EE5E7BA37}" name="cod_escuela"/>
-    <tableColumn id="8" xr3:uid="{FB89F258-CC9C-452F-A80B-887C2E6D6E47}" name="cod_plan"/>
-    <tableColumn id="9" xr3:uid="{31EDA648-E658-4798-9160-C41304C7164F}" name="cod_semestre"/>
-    <tableColumn id="10" xr3:uid="{94423EF1-4680-43B6-8401-8C2116F1674C}" name="cod_especialidad"/>
-    <tableColumn id="11" xr3:uid="{3080F490-B170-496C-BEEB-C8FFF0E6D924}" name="ind_estado_acta"/>
-    <tableColumn id="12" xr3:uid="{8EE73639-AB7F-4927-9BC3-6BE36CA9A5C7}" name="aula_turno"/>
-    <tableColumn id="13" xr3:uid="{0B37BBBD-9259-4E30-B362-6D75CE34B11F}" name="can_alum_matriculados"/>
-    <tableColumn id="14" xr3:uid="{68EE8755-BC9F-4772-8C68-10063BEFD917}" name="num_ciclo_ano_asignatura"/>
-    <tableColumn id="15" xr3:uid="{9073CE89-017A-4E0F-9046-92FA3890E92D}" name="ind_semestre_par"/>
-    <tableColumn id="16" xr3:uid="{C5C656A3-BADD-4DE1-8B76-1641FB7154F5}" name="num_creditaje"/>
-    <tableColumn id="17" xr3:uid="{3FC67CBB-15D7-45D0-BC4A-E09B0E5EC1BF}" name="des_asignatura"/>
-    <tableColumn id="18" xr3:uid="{77170B83-9BCE-4A21-9254-B55887D16AA3}" name="cod_grupo"/>
-    <tableColumn id="19" xr3:uid="{F179CEFD-839C-44A8-A2C9-EED4DA26977B}" name="des_plan"/>
-    <tableColumn id="20" xr3:uid="{077A7D18-3590-4655-9A47-758997DB25D3}" name="ind_reg_plan"/>
-    <tableColumn id="21" xr3:uid="{BDB7BFF2-7D00-4005-84B3-FEFCEDF6B54D}" name="des_especialidad"/>
-    <tableColumn id="22" xr3:uid="{813AF850-CBAE-4913-8A27-344223CECFB3}" name="ape_paterno"/>
-    <tableColumn id="23" xr3:uid="{6FD8A5C5-2D13-4EFA-83F5-458264244EE5}" name="ape_materno"/>
-    <tableColumn id="24" xr3:uid="{F30B69AE-EBE8-455C-AA7E-03B99DC433FF}" name="nom_docente"/>
-    <tableColumn id="25" xr3:uid="{21DBC12D-37FC-4826-AF96-28567AEFF73B}" name="t_especialidad"/>
-    <tableColumn id="26" xr3:uid="{1A873F28-5387-4322-B6CF-49C48198F6D5}" name="des_grupo"/>
-    <tableColumn id="27" xr3:uid="{45C7BFAF-6A0C-4FFA-9F7B-CB2D0CFF3A00}" name="des_dictado"/>
-    <tableColumn id="28" xr3:uid="{C9CAABBB-0C87-449E-B4F9-5BC2F9074465}" name="sede_seccion"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Quotable">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
-    <a:clrScheme name="Blue Warm">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -470,48 +413,83 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="242852"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="ACCBF9"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4A66AC"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="629DD1"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="297FD5"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="7F8FA9"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5AA2AE"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="9D90A0"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="9454C3"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="3EBBF0"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Quotable">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Century Gothic" panose="020B0502020202020204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Tahoma"/>
-        <a:font script="Hebr" typeface="Gisha"/>
-        <a:font script="Thai" typeface="DilleniaUPC"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
         <a:font script="Ethi" typeface="Nyala"/>
         <a:font script="Beng" typeface="Vrinda"/>
         <a:font script="Gujr" typeface="Shruti"/>
@@ -532,47 +510,12 @@
         <a:font script="Laoo" typeface="DokChampa"/>
         <a:font script="Sinh" typeface="Iskoola Pota"/>
         <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Tahoma"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Century Gothic" panose="020B0502020202020204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Tahoma"/>
-        <a:font script="Hebr" typeface="Gisha"/>
-        <a:font script="Thai" typeface="DilleniaUPC"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Verdana"/>
+        <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Quotable">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -581,52 +524,76 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
                 <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="90000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:blipFill rotWithShape="1">
-          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-            <a:duotone>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
+                <a:satMod val="103000"/>
                 <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
               </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:shade val="98000"/>
-                <a:lumMod val="98000"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
-            </a:duotone>
-          </a:blip>
-          <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
-        </a:blipFill>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="rnd" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="15875" cap="rnd" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="25400" cap="rnd" cmpd="sng" algn="ctr">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -638,11 +605,11 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:innerShdw blurRad="63500" dist="25400" dir="13500000">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="75000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
-            </a:innerShdw>
+            </a:outerShdw>
           </a:effectLst>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -650,35 +617,35 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="84000"/>
-                <a:shade val="84000"/>
-                <a:lumMod val="90000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="84000"/>
-                <a:shade val="90000"/>
-                <a:satMod val="120000"/>
-                <a:lumMod val="90000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr"/>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
@@ -690,51 +657,19 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Quotable" id="{39EC5628-30ED-4578-ACD8-9820EDB8E15A}" vid="{6F3559E9-1A4C-49D8-94D4-F41003531C49}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="18.140625" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="25.28515625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.5703125" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="16.42578125" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="63.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.85546875" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="20" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="15.140625" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="19.140625" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.5703125" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="12.7109375" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="14.140625" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="15.5703125" hidden="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -860,7 +795,7 @@
         <v>34</v>
       </c>
       <c r="M2">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="N2">
         <v>1</v>
@@ -904,13 +839,13 @@
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
         <v>29</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
         <v>30</v>
@@ -937,10 +872,10 @@
         <v>33</v>
       </c>
       <c r="L3" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="M3">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="N3">
         <v>1</v>
@@ -952,7 +887,7 @@
         <v>3</v>
       </c>
       <c r="Q3" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="S3" t="s">
         <v>37</v>
@@ -964,13 +899,13 @@
         <v>39</v>
       </c>
       <c r="V3" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="W3" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="X3" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="Y3" t="s">
         <v>43</v>
@@ -984,7 +919,7 @@
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s">
         <v>29</v>
@@ -1020,7 +955,7 @@
         <v>51</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="N4">
         <v>1</v>
@@ -1032,7 +967,7 @@
         <v>3</v>
       </c>
       <c r="Q4" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="S4" t="s">
         <v>37</v>
@@ -1044,13 +979,13 @@
         <v>39</v>
       </c>
       <c r="V4" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="W4" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="X4" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="Y4" t="s">
         <v>43</v>
@@ -1064,13 +999,13 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
         <v>29</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
         <v>30</v>
@@ -1097,10 +1032,10 @@
         <v>33</v>
       </c>
       <c r="L5" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="N5">
         <v>1</v>
@@ -1112,7 +1047,7 @@
         <v>3</v>
       </c>
       <c r="Q5" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="S5" t="s">
         <v>37</v>
@@ -1122,6 +1057,15 @@
       </c>
       <c r="U5" t="s">
         <v>39</v>
+      </c>
+      <c r="V5" t="s">
+        <v>57</v>
+      </c>
+      <c r="W5" t="s">
+        <v>58</v>
+      </c>
+      <c r="X5" t="s">
+        <v>59</v>
       </c>
       <c r="Y5" t="s">
         <v>43</v>
@@ -1135,7 +1079,7 @@
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="B6" t="s">
         <v>29</v>
@@ -1171,7 +1115,7 @@
         <v>51</v>
       </c>
       <c r="M6">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="N6">
         <v>1</v>
@@ -1183,7 +1127,7 @@
         <v>3</v>
       </c>
       <c r="Q6" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="S6" t="s">
         <v>37</v>
@@ -1195,13 +1139,13 @@
         <v>39</v>
       </c>
       <c r="V6" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="W6" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="X6" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="Y6" t="s">
         <v>43</v>
@@ -1215,13 +1159,13 @@
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
         <v>29</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D7" t="s">
         <v>30</v>
@@ -1248,10 +1192,10 @@
         <v>33</v>
       </c>
       <c r="L7" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="M7">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="N7">
         <v>1</v>
@@ -1263,7 +1207,7 @@
         <v>3</v>
       </c>
       <c r="Q7" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="S7" t="s">
         <v>37</v>
@@ -1273,15 +1217,6 @@
       </c>
       <c r="U7" t="s">
         <v>39</v>
-      </c>
-      <c r="V7" t="s">
-        <v>77</v>
-      </c>
-      <c r="W7" t="s">
-        <v>78</v>
-      </c>
-      <c r="X7" t="s">
-        <v>79</v>
       </c>
       <c r="Y7" t="s">
         <v>43</v>
@@ -1295,7 +1230,7 @@
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="B8" t="s">
         <v>29</v>
@@ -1331,7 +1266,7 @@
         <v>51</v>
       </c>
       <c r="M8">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="N8">
         <v>1</v>
@@ -1343,7 +1278,7 @@
         <v>3</v>
       </c>
       <c r="Q8" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
       <c r="S8" t="s">
         <v>37</v>
@@ -1353,15 +1288,6 @@
       </c>
       <c r="U8" t="s">
         <v>39</v>
-      </c>
-      <c r="V8" t="s">
-        <v>82</v>
-      </c>
-      <c r="W8" t="s">
-        <v>83</v>
-      </c>
-      <c r="X8" t="s">
-        <v>84</v>
       </c>
       <c r="Y8" t="s">
         <v>43</v>
@@ -1375,7 +1301,7 @@
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
         <v>29</v>
@@ -1408,10 +1334,10 @@
         <v>33</v>
       </c>
       <c r="L9" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="M9">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="N9">
         <v>1</v>
@@ -1423,7 +1349,7 @@
         <v>3</v>
       </c>
       <c r="Q9" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="S9" t="s">
         <v>37</v>
@@ -1435,13 +1361,13 @@
         <v>39</v>
       </c>
       <c r="V9" t="s">
-        <v>47</v>
+        <v>67</v>
       </c>
       <c r="W9" t="s">
-        <v>48</v>
+        <v>68</v>
       </c>
       <c r="X9" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="Y9" t="s">
         <v>43</v>
@@ -1455,13 +1381,13 @@
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="B10" t="s">
         <v>29</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" t="s">
         <v>30</v>
@@ -1488,10 +1414,10 @@
         <v>33</v>
       </c>
       <c r="L10" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="M10">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="N10">
         <v>1</v>
@@ -1503,7 +1429,7 @@
         <v>3</v>
       </c>
       <c r="Q10" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="S10" t="s">
         <v>37</v>
@@ -1515,13 +1441,13 @@
         <v>39</v>
       </c>
       <c r="V10" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="W10" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="X10" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="Y10" t="s">
         <v>43</v>
@@ -1535,7 +1461,7 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="B11" t="s">
         <v>29</v>
@@ -1568,10 +1494,10 @@
         <v>33</v>
       </c>
       <c r="L11" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="M11">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="N11">
         <v>1</v>
@@ -1583,7 +1509,7 @@
         <v>3</v>
       </c>
       <c r="Q11" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="S11" t="s">
         <v>37</v>
@@ -1606,13 +1532,13 @@
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="B12" t="s">
         <v>29</v>
       </c>
       <c r="C12">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D12" t="s">
         <v>30</v>
@@ -1639,10 +1565,10 @@
         <v>33</v>
       </c>
       <c r="L12" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="M12">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="N12">
         <v>1</v>
@@ -1654,7 +1580,7 @@
         <v>3</v>
       </c>
       <c r="Q12" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="S12" t="s">
         <v>37</v>
@@ -1666,13 +1592,13 @@
         <v>39</v>
       </c>
       <c r="V12" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="W12" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="X12" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="Y12" t="s">
         <v>43</v>
@@ -1686,7 +1612,7 @@
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
         <v>29</v>
@@ -1722,7 +1648,7 @@
         <v>56</v>
       </c>
       <c r="M13">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="N13">
         <v>1</v>
@@ -1734,7 +1660,7 @@
         <v>3</v>
       </c>
       <c r="Q13" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="S13" t="s">
         <v>37</v>
@@ -1757,13 +1683,13 @@
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B14" t="s">
         <v>29</v>
       </c>
       <c r="C14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D14" t="s">
         <v>30</v>
@@ -1790,10 +1716,10 @@
         <v>33</v>
       </c>
       <c r="L14" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="M14">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="N14">
         <v>1</v>
@@ -1805,7 +1731,7 @@
         <v>3</v>
       </c>
       <c r="Q14" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="S14" t="s">
         <v>37</v>
@@ -1815,6 +1741,15 @@
       </c>
       <c r="U14" t="s">
         <v>39</v>
+      </c>
+      <c r="V14" t="s">
+        <v>82</v>
+      </c>
+      <c r="W14" t="s">
+        <v>83</v>
+      </c>
+      <c r="X14" t="s">
+        <v>84</v>
       </c>
       <c r="Y14" t="s">
         <v>43</v>
@@ -1864,7 +1799,7 @@
         <v>56</v>
       </c>
       <c r="M15">
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="N15">
         <v>1</v>
@@ -1908,8 +1843,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
 </worksheet>
 </file>
</xml_diff>